<commit_message>
Project is updated with some more details
</commit_message>
<xml_diff>
--- a/testdata/TestData.xlsx
+++ b/testdata/TestData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kiran\eclipse-workspace\OpenCart_V121_Artifact_ID\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3823D27-0564-499D-9F53-C3B0053AD911}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD758FB2-5E98-47EF-8628-D11080670A7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{F4F91135-86BC-47E8-9F2E-52A4897173F9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="18">
   <si>
     <t>Username</t>
   </si>
@@ -81,13 +81,22 @@
   </si>
   <si>
     <t>SrL@wv</t>
+  </si>
+  <si>
+    <t>uaaxv@gmail.com</t>
+  </si>
+  <si>
+    <t>LWW@Ujt</t>
+  </si>
+  <si>
+    <t>LWW@Uj</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -128,6 +137,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF2A00FF"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -156,13 +172,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -568,10 +586,15 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
@@ -585,44 +608,44 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>3</v>
+      <c r="A2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>13</v>
+      <c r="A3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>7</v>
+      <c r="A4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>14</v>
+      <c r="A5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>10</v>
@@ -630,8 +653,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{C2C8B901-1810-48F9-8888-3BCDA505CCF2}"/>
-    <hyperlink ref="B5" r:id="rId2" xr:uid="{D9879DB6-B951-4210-9897-7F0A3F77F463}"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{E864E7F2-1169-4319-ADCA-46AB8A011672}"/>
+    <hyperlink ref="B5" r:id="rId2" xr:uid="{E6BE8BAF-B653-45D1-807E-5CF992E05EDF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>